<commit_message>
Updated code for bugfixes. Also added example outputs and plots for this parameter estimation run from our local cluster: Caviness.
</commit_message>
<xml_diff>
--- a/examples/omkm_interface/omkm_petbo_run/inputs/NH3_Input_Data.xlsx
+++ b/examples/omkm_interface/omkm_petbo_run/inputs/NH3_Input_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skasiraj\source\repos\Parameter-Estimation-BO\examples\omkm_interface\omkm-petbo\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skasiraj\source\repos\Parameter-Estimation-BO\examples\omkm_interface\omkm_petbo_run\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630B2B14-29FE-403D-AC0B-3A0D5CDA1FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E61C5DB-7EE6-458E-9E9F-0BD5CD6F146F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="9" r:id="rId1"/>
@@ -6033,7 +6033,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6141,7 +6141,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>